<commit_message>
add missing tables to AACT_Tables spreadsheet
</commit_message>
<xml_diff>
--- a/public/documentation/aact_tables.xlsx
+++ b/public/documentation/aact_tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="15140" tabRatio="500"/>
+    <workbookView xWindow="3660" yWindow="1580" windowWidth="22460" windowHeight="12920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="AACT Tables and Columns" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,414 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="137">
+  <si>
+    <t>Description of planned outcome measures and observations that will describe patterns of diseases and traits/associations with exposures, risk factors or treatment.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OutcomesBody</t>
+  </si>
+  <si>
+    <t>StudyDesignLabel</t>
+  </si>
+  <si>
+    <t>Detailed_Descriptions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A single text column that provides a detailed description of the study protocol.</t>
+  </si>
+  <si>
+    <t>DetailedDescription</t>
+  </si>
+  <si>
+    <t>Drop_Withdrawals</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mesh_Headings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mesh_Terms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contains the content of the 2016 MeSH terms published by the National Library of Medicine.  These values are used in Browse_Conditions &amp; Browse_Interventions table, however this and the Mesh_Headings table are the only 2 tables that do not relate directly to the Studies table.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n/a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n/a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides MeSH headings &amp; subheadings.  Rows do not directly relate to Studies from ClinicalTrials.gov.  This is a table to support investigators who use MeSH terms. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Summaries of demographic &amp; baseline measures collected by arm or comparison group and for the entire population of participants in the clinical study. </t>
+  </si>
+  <si>
+    <t>BaselineUnitOfMeasure</t>
+  </si>
+  <si>
+    <t>A single text column that provides a brief description of the study.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>Provides words or phrases that best describe the protocol. Keywords help users find studies in the database. Can include NLM's Medical Subject Heading (MeSH)-controlled vocabulary terms.</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>Links</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Web site directly relevant to the protocol.  (ie, links to educational, research, government, and other non-profit Web pages)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>BriefSummary</t>
+  </si>
+  <si>
+    <t>NLM uses an internal algorithm to assess the data entered for a study and creates a list of standard MeSH terms that describe the condition(s) being addressed by the clinical trial.  This table provides the results of NLM's assessment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Browse_Interventions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NLM uses an internal algorithm to assess the data entered for a study and creates a list of standard MeSH terms that describe the intervention(s) being addressed by the clinical trial.  This table provides the results of NLM's assessment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>An AACT-provided table that contains info that's been calculated from the information received from ClinicalTrials.gov.  For example, number_of_facilities and actual_duration are provided in this table.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contact info for people (primary &amp; backup) who can answer questions concerning enrollment at any location of the study.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name(s) of the disease(s) or condition(s) studied in the clinical study, or the focus of the clinical study. Can include NLM's Medical Subject Heading (MeSH)-controlled vocabulary terms.</t>
+  </si>
+  <si>
+    <t>Defines the protocol-specified group, subgroup, or cohort of participants in a clinical trial assigned to receive specific intervention(s) or observations according to a protocol.</t>
+  </si>
+  <si>
+    <t>ArmsGroupsInterventionsLabel</t>
+  </si>
+  <si>
+    <t>Descriptions of outcomes, or observation that were measured to determine patterns of diseases or traits, or associations with exposures, risk factors, or treatment. Includes information such as time frame, population and units.  (Specific measurement results are stored in the Outcome_Measurements table.)</t>
+  </si>
+  <si>
+    <t>Result_Outcome_MeasureImg</t>
+  </si>
+  <si>
+    <t>Facilities</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Facility_Contacts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Facility_Investigators</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Id_Information</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intervention_Other_Names</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interventions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Keywords</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Milestones</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outcome_Analyses</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outcome_Analysis_Groups</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overall_Officials</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>People responsible for the overall scientific leadership of the protocol including the principal investigator.</t>
+  </si>
+  <si>
+    <t>Summarized information about how many participants withdrew from the study, when and why. This information explains disposition of participants relative to the numbers starting and completing the study (enumerated in the Milestones table).</t>
+  </si>
+  <si>
+    <t>NotCompleted</t>
+  </si>
+  <si>
+    <t>Eligibilities</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Information about the criteria used to select participants; includes inclusion and exclusion criteria</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EligibilityLabel</t>
+  </si>
+  <si>
+    <t>Name, address and recruiting status of the facilities participating in the study.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Facility</t>
+  </si>
+  <si>
+    <t>Contact information for people responsible for the study at each facility. (primary and backup)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FacilityContact</t>
+  </si>
+  <si>
+    <t>Names of the investigators at each study facility.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StudyOfficials</t>
+  </si>
+  <si>
+    <t>Sample size at baseline for each study group; usually a count of participants but can represent other units of measure such as 'hands', 'hips', etc.</t>
+  </si>
+  <si>
+    <t>many</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>The interventions or exposures (including drugs, medical devices, procedures, vaccines, and other products) of interest to the study, or associated with study arms/groups.</t>
+  </si>
+  <si>
+    <t>IntDesign</t>
+  </si>
+  <si>
+    <t>Result_Baseline_ArmGroup_numUnitsAnalyzed</t>
+  </si>
+  <si>
+    <t>Info about whether an agreement exists between the sponsor &amp; the principal investigators (PIs) that restricts the PIs ability to discuss study results at scientific meetings or other public or private forums, or to publish info concerning the study in scientific or academic journals after the study is completed.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result_CertainAgreementLabel</t>
+  </si>
+  <si>
+    <t>Outcome_Counts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outcome_Measurements</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outcomes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Participant_Flows</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reported_Events</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Responsible_Parties</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result_Agreements</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result_Contacts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result_Groups</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sponsors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Studies</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rows per study</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>db section</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nlm doc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Information summarizing the progress of participants through each stage of a study, including the number of participants who started and completed the trial. Enumeration of participants not completing the study is included in the Drop_Withdrawals table.</t>
+  </si>
+  <si>
+    <t>MilestoneName</t>
+  </si>
+  <si>
+    <t>Results of scientifically appropriate statistical analyses performed on primary and secondary study outcomes. Includes results for treatment effect estimates, confidence intervals and othe rmeasures of dispersion, and p-values.</t>
+  </si>
+  <si>
+    <t>Result_Outcome_Analysis</t>
+  </si>
+  <si>
+    <t>Identifies the comparison groups that were involved with each outcome analysis</t>
+  </si>
+  <si>
+    <t>GroupSelection</t>
+  </si>
+  <si>
+    <t>Sample size included in analysis for each outcome for each study group; usually participants but can represent other units of measure such as eyes 'lesions', etc.</t>
+  </si>
+  <si>
+    <t>OutcomeData</t>
+  </si>
+  <si>
+    <t>Countries in which the study has facilities/sites.</t>
+  </si>
+  <si>
+    <t>A cross reference for groups/interventions.  If a study has multiple groups and multiple interventions, this table shows which interventions are associated with which groups.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>many</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crossref</t>
+  </si>
+  <si>
+    <t>Design_Groups</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Calculated_Values</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Central_Contacts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Conditions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Countries</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Design_Group_Interventions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Design_Outcomes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Designs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IPD_Information_Types</t>
+  </si>
+  <si>
+    <t>The type(s) of supporting information that will be shared, in addition to the individual participant data set and data dictionaries for the IPD itself. Select all that apply:  Study Protocol, Statistical Analysis Plan (SAP), Informed Consent Form (ICF), Clinical Study Report (CSR), Analytic Code</t>
+  </si>
+  <si>
+    <t>IPDSharing</t>
+  </si>
+  <si>
+    <t>Recruitment information relevant to the recruitment process &amp; pre-assignment details (ie. significant events in the study that occur after participant enrollment, but prior to assignment of participants).  Information about participant flow that applies to all milestones.</t>
+  </si>
+  <si>
+    <t>Result_ParticipantFlowLabel</t>
+  </si>
+  <si>
+    <t>Summary information about reported adverse events (any untoward or unfavorable medical occurrence to participants, including abnormal physical exams, laboratory findings, symptoms, or diseases), including serious adverse events, other adverse events, and mortality.</t>
+  </si>
+  <si>
+    <t>Result_AdverseEventsLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People who have access to and control over the data from the study, have the right to publish study results, and have the ability to meet all of the requirements for the submission of study information. </t>
+  </si>
+  <si>
+    <t>RespParty</t>
+  </si>
+  <si>
+    <t>Identifiers (other than the NCT ID) that uniquely identify the study such as that assigned by the sponsor, or an NCT ID that had previously been used for the study.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SecondaryIds</t>
+  </si>
+  <si>
+    <t>Terns or phrases that are synonymous with an intervention.  (Each row is linked to one of the interventions associated with the study.)</t>
+  </si>
+  <si>
+    <t>InterventionOtherName</t>
+  </si>
   <si>
     <t>DocumentUpload</t>
   </si>
@@ -96,389 +503,6 @@
   </si>
   <si>
     <t>Browse_Conditions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Calculated_Values</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Central_Contacts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Conditions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Countries</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Design_Group_Interventions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Design_Outcomes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Designs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IPD_Information_Types</t>
-  </si>
-  <si>
-    <t>The type(s) of supporting information that will be shared, in addition to the individual participant data set and data dictionaries for the IPD itself. Select all that apply:  Study Protocol, Statistical Analysis Plan (SAP), Informed Consent Form (ICF), Clinical Study Report (CSR), Analytic Code</t>
-  </si>
-  <si>
-    <t>IPDSharing</t>
-  </si>
-  <si>
-    <t>Recruitment information relevant to the recruitment process &amp; pre-assignment details (ie. significant events in the study that occur after participant enrollment, but prior to assignment of participants).  Information about participant flow that applies to all milestones.</t>
-  </si>
-  <si>
-    <t>Result_ParticipantFlowLabel</t>
-  </si>
-  <si>
-    <t>Summary information about reported adverse events (any untoward or unfavorable medical occurrence to participants, including abnormal physical exams, laboratory findings, symptoms, or diseases), including serious adverse events, other adverse events, and mortality.</t>
-  </si>
-  <si>
-    <t>Result_AdverseEventsLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">People who have access to and control over the data from the study, have the right to publish study results, and have the ability to meet all of the requirements for the submission of study information. </t>
-  </si>
-  <si>
-    <t>RespParty</t>
-  </si>
-  <si>
-    <t>Identifiers (other than the NCT ID) that uniquely identify the study such as that assigned by the sponsor, or an NCT ID that had previously been used for the study.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SecondaryIds</t>
-  </si>
-  <si>
-    <t>Terns or phrases that are synonymous with an intervention.  (Each row is linked to one of the interventions associated with the study.)</t>
-  </si>
-  <si>
-    <t>InterventionOtherName</t>
-  </si>
-  <si>
-    <t>Info about whether an agreement exists between the sponsor &amp; the principal investigators (PIs) that restricts the PIs ability to discuss study results at scientific meetings or other public or private forums, or to publish info concerning the study in scientific or academic journals after the study is completed.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Result_CertainAgreementLabel</t>
-  </si>
-  <si>
-    <t>Outcome_Counts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Outcome_Measurements</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Outcomes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Participant_Flows</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reported_Events</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Responsible_Parties</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Result_Agreements</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Result_Contacts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Result_Groups</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sponsors</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Studies</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rows per study</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>db section</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nlm doc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Information summarizing the progress of participants through each stage of a study, including the number of participants who started and completed the trial. Enumeration of participants not completing the study is included in the Drop_Withdrawals table.</t>
-  </si>
-  <si>
-    <t>MilestoneName</t>
-  </si>
-  <si>
-    <t>Results of scientifically appropriate statistical analyses performed on primary and secondary study outcomes. Includes results for treatment effect estimates, confidence intervals and othe rmeasures of dispersion, and p-values.</t>
-  </si>
-  <si>
-    <t>Result_Outcome_Analysis</t>
-  </si>
-  <si>
-    <t>Identifies the comparison groups that were involved with each outcome analysis</t>
-  </si>
-  <si>
-    <t>GroupSelection</t>
-  </si>
-  <si>
-    <t>Sample size included in analysis for each outcome for each study group; usually participants but can represent other units of measure such as eyes 'lesions', etc.</t>
-  </si>
-  <si>
-    <t>OutcomeData</t>
-  </si>
-  <si>
-    <t>Countries in which the study has facilities/sites.</t>
-  </si>
-  <si>
-    <t>A cross reference for groups/interventions.  If a study has multiple groups and multiple interventions, this table shows which interventions are associated with which groups.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>many</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>crossref</t>
-  </si>
-  <si>
-    <t>Design_Groups</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Descriptions of outcomes, or observation that were measured to determine patterns of diseases or traits, or associations with exposures, risk factors, or treatment. Includes information such as time frame, population and units.  (Specific measurement results are stored in the Outcome_Measurements table.)</t>
-  </si>
-  <si>
-    <t>Result_Outcome_MeasureImg</t>
-  </si>
-  <si>
-    <t>Facilities</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Facility_Contacts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Facility_Investigators</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Id_Information</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intervention_Other_Names</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interventions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Keywords</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Milestones</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Outcome_Analyses</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Outcome_Analysis_Groups</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overall_Officials</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>People responsible for the overall scientific leadership of the protocol including the principal investigator.</t>
-  </si>
-  <si>
-    <t>Summarized information about how many participants withdrew from the study, when and why. This information explains disposition of participants relative to the numbers starting and completing the study (enumerated in the Milestones table).</t>
-  </si>
-  <si>
-    <t>NotCompleted</t>
-  </si>
-  <si>
-    <t>Eligibilities</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Information about the criteria used to select participants; includes inclusion and exclusion criteria</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EligibilityLabel</t>
-  </si>
-  <si>
-    <t>Name, address and recruiting status of the facilities participating in the study.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Facility</t>
-  </si>
-  <si>
-    <t>Contact information for people responsible for the study at each facility. (primary and backup)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FacilityContact</t>
-  </si>
-  <si>
-    <t>Names of the investigators at each study facility.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StudyOfficials</t>
-  </si>
-  <si>
-    <t>Sample size at baseline for each study group; usually a count of participants but can represent other units of measure such as 'hands', 'hips', etc.</t>
-  </si>
-  <si>
-    <t>many</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>The interventions or exposures (including drugs, medical devices, procedures, vaccines, and other products) of interest to the study, or associated with study arms/groups.</t>
-  </si>
-  <si>
-    <t>IntDesign</t>
-  </si>
-  <si>
-    <t>Result_Baseline_ArmGroup_numUnitsAnalyzed</t>
-  </si>
-  <si>
-    <t>Summaries of demographic &amp; baseline measures collected by arm or comparison group and for the entire population of participants in the clinical study. </t>
-  </si>
-  <si>
-    <t>BaselineUnitOfMeasure</t>
-  </si>
-  <si>
-    <t>A single text column that provides a brief description of the study.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>one</t>
-  </si>
-  <si>
-    <t>Protocol</t>
-  </si>
-  <si>
-    <t>Provides words or phrases that best describe the protocol. Keywords help users find studies in the database. Can include NLM's Medical Subject Heading (MeSH)-controlled vocabulary terms.</t>
-  </si>
-  <si>
-    <t>Keywords</t>
-  </si>
-  <si>
-    <t>Links</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Web site directly relevant to the protocol.  (ie, links to educational, research, government, and other non-profit Web pages)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Links</t>
-  </si>
-  <si>
-    <t>BriefSummary</t>
-  </si>
-  <si>
-    <t>NLM uses an internal algorithm to assess the data entered for a study and creates a list of standard MeSH terms that describe the condition(s) being addressed by the clinical trial.  This table provides the results of NLM's assessment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Browse_Interventions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NLM uses an internal algorithm to assess the data entered for a study and creates a list of standard MeSH terms that describe the intervention(s) being addressed by the clinical trial.  This table provides the results of NLM's assessment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>An AACT-provided table that contains info that's been calculated from the information received from ClinicalTrials.gov.  For example, number_of_facilities and actual_duration are provided in this table.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Contact info for people (primary &amp; backup) who can answer questions concerning enrollment at any location of the study.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name(s) of the disease(s) or condition(s) studied in the clinical study, or the focus of the clinical study. Can include NLM's Medical Subject Heading (MeSH)-controlled vocabulary terms.</t>
-  </si>
-  <si>
-    <t>Defines the protocol-specified group, subgroup, or cohort of participants in a clinical trial assigned to receive specific intervention(s) or observations according to a protocol.</t>
-  </si>
-  <si>
-    <t>ArmsGroupsInterventionsLabel</t>
-  </si>
-  <si>
-    <t>Description of planned outcome measures and observations that will describe patterns of diseases and traits/associations with exposures, risk factors or treatment.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OutcomesBody</t>
-  </si>
-  <si>
-    <t>StudyDesignLabel</t>
-  </si>
-  <si>
-    <t>Detailed_Descriptions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A single text column that provides a detailed description of the study protocol.</t>
-  </si>
-  <si>
-    <t>DetailedDescription</t>
-  </si>
-  <si>
-    <t>Drop_Withdrawals</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -486,12 +510,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="14">
     <font>
       <sz val="10"/>
@@ -689,7 +707,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>233</xdr:row>
+      <xdr:row>235</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184666" cy="261610"/>
@@ -698,7 +716,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1063,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E272"/>
+  <dimension ref="A1:E274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -1081,733 +1099,751 @@
   <sheetData>
     <row r="1" spans="1:5" s="12" customFormat="1">
       <c r="A1" s="12" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="39">
       <c r="A2" s="13" t="s">
-        <v>18</v>
+        <v>133</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="45">
       <c r="A3" s="13" t="s">
-        <v>19</v>
+        <v>134</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>104</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="14" t="s">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>114</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="60">
       <c r="A5" s="14" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="60">
       <c r="A6" s="14" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45">
       <c r="A7" s="14" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30">
       <c r="A8" s="14" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>120</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45">
       <c r="A9" s="14" t="s">
-        <v>24</v>
+        <v>97</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>121</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>120</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="14" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>120</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45">
       <c r="A11" s="14" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45">
       <c r="A12" s="14" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>122</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>123</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45">
       <c r="A13" s="14" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>124</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30">
       <c r="A14" s="14" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="14" t="s">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>128</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>129</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="20" customFormat="1">
       <c r="A16" s="19" t="s">
-        <v>3</v>
+        <v>118</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>1</v>
+        <v>116</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>4</v>
+        <v>119</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="3" customFormat="1" ht="60">
       <c r="A17" s="13" t="s">
-        <v>130</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30">
       <c r="A18" s="14" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="14" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30">
       <c r="A20" s="14" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="14" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="45">
       <c r="A22" s="14" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30">
       <c r="A23" s="14" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="45">
       <c r="A24" s="14" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="60">
       <c r="A25" s="14" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="45">
       <c r="A26" s="14" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>109</v>
+        <v>18</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>110</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30">
       <c r="A27" s="14" t="s">
-        <v>111</v>
+        <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" ht="60">
-      <c r="A28" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45">
+      <c r="A28" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" ht="60">
+      <c r="A29" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" s="3" customFormat="1" ht="60">
+      <c r="A30" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="C30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="3" customFormat="1" ht="45">
-      <c r="A29" s="13" t="s">
+      <c r="E30" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="3" customFormat="1" ht="30">
-      <c r="A30" s="13" t="s">
+    </row>
+    <row r="31" spans="1:5" s="3" customFormat="1" ht="45">
+      <c r="A31" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="3" customFormat="1" ht="30">
-      <c r="A31" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="3" customFormat="1" ht="30">
       <c r="A32" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="3" customFormat="1" ht="60">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="3" customFormat="1" ht="30">
       <c r="A33" s="13" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="30">
-      <c r="A34" s="14" t="s">
-        <v>85</v>
+        <v>60</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="3" customFormat="1" ht="30">
+      <c r="A34" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>97</v>
+        <v>59</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="3" customFormat="1" ht="60">
       <c r="A35" s="13" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30">
+      <c r="A36" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="3" customFormat="1" ht="60">
+      <c r="A37" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="3" customFormat="1" ht="60">
+      <c r="A38" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="3" customFormat="1" ht="60">
-      <c r="A36" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="45">
-      <c r="A37" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="C38" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E37" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="3" customFormat="1" ht="75">
-      <c r="A38" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="3" customFormat="1" ht="30">
-      <c r="A39" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>6</v>
+    </row>
+    <row r="39" spans="1:5" ht="45">
+      <c r="A39" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="3" customFormat="1" ht="30">
+        <v>59</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="3" customFormat="1" ht="75">
       <c r="A40" s="13" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="52">
-      <c r="A41" s="14" t="s">
-        <v>53</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="3" customFormat="1" ht="30">
+      <c r="A41" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="60">
-      <c r="A42" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>12</v>
+        <v>59</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="3" customFormat="1" ht="30">
+      <c r="A42" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="9"/>
-    </row>
-    <row r="43" spans="1:5" ht="30">
+        <v>59</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="52">
       <c r="A43" s="14" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>15</v>
+        <v>125</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E43" s="8"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="E45" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="60">
+      <c r="A44" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E44" s="9"/>
+    </row>
+    <row r="45" spans="1:5" ht="30">
+      <c r="A45" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2"/>
@@ -1821,20 +1857,20 @@
       <c r="C47" s="2"/>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:5" s="5" customFormat="1"/>
-    <row r="49" spans="1:5" s="5" customFormat="1"/>
-    <row r="50" spans="1:5">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="E51" s="2"/>
-    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" s="5" customFormat="1"/>
+    <row r="51" spans="1:5" s="5" customFormat="1"/>
     <row r="52" spans="1:5">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
@@ -1883,21 +1919,21 @@
       <c r="C59" s="2"/>
       <c r="E59" s="2"/>
     </row>
-    <row r="60" spans="1:5" s="3" customFormat="1"/>
-    <row r="61" spans="1:5" s="5" customFormat="1"/>
-    <row r="62" spans="1:5" s="5" customFormat="1"/>
-    <row r="63" spans="1:5">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="E63" s="2"/>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="E64" s="2"/>
-    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="1:5" s="3" customFormat="1"/>
+    <row r="63" spans="1:5" s="5" customFormat="1"/>
+    <row r="64" spans="1:5" s="5" customFormat="1"/>
     <row r="65" spans="1:5">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
@@ -1922,39 +1958,39 @@
       <c r="C68" s="2"/>
       <c r="E68" s="2"/>
     </row>
-    <row r="69" spans="1:5" s="3" customFormat="1"/>
-    <row r="70" spans="1:5" s="3" customFormat="1"/>
-    <row r="71" spans="1:5">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="E71" s="2"/>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="E72" s="2"/>
-    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="1:5" s="3" customFormat="1"/>
+    <row r="72" spans="1:5" s="3" customFormat="1"/>
     <row r="73" spans="1:5">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="E73" s="2"/>
     </row>
-    <row r="74" spans="1:5" s="3" customFormat="1"/>
+    <row r="74" spans="1:5">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="E74" s="2"/>
+    </row>
     <row r="75" spans="1:5">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="E75" s="2"/>
     </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="E76" s="2"/>
-    </row>
+    <row r="76" spans="1:5" s="3" customFormat="1"/>
     <row r="77" spans="1:5">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
@@ -1962,9 +1998,15 @@
       <c r="E77" s="2"/>
     </row>
     <row r="78" spans="1:5">
+      <c r="A78" s="2"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
       <c r="E78" s="2"/>
     </row>
     <row r="79" spans="1:5">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
       <c r="E79" s="2"/>
     </row>
     <row r="80" spans="1:5">
@@ -1985,10 +2027,8 @@
     <row r="85" spans="1:5">
       <c r="E85" s="2"/>
     </row>
-    <row r="86" spans="1:5" s="3" customFormat="1">
-      <c r="A86" s="16"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
+    <row r="86" spans="1:5">
+      <c r="E86" s="2"/>
     </row>
     <row r="87" spans="1:5">
       <c r="E87" s="2"/>
@@ -1998,16 +2038,18 @@
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="1:5" s="3" customFormat="1">
-      <c r="A89" s="16"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="1:5">
-      <c r="E90" s="2"/>
-    </row>
-    <row r="91" spans="1:5">
-      <c r="E91" s="2"/>
+    <row r="89" spans="1:5">
+      <c r="E89" s="2"/>
+    </row>
+    <row r="90" spans="1:5" s="3" customFormat="1">
+      <c r="A90" s="16"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+    </row>
+    <row r="91" spans="1:5" s="3" customFormat="1">
+      <c r="A91" s="16"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
     </row>
     <row r="92" spans="1:5">
       <c r="E92" s="2"/>
@@ -2039,16 +2081,16 @@
     <row r="101" spans="1:5">
       <c r="E101" s="2"/>
     </row>
-    <row r="102" spans="1:5" s="3" customFormat="1">
-      <c r="A102" s="16"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
+    <row r="102" spans="1:5">
+      <c r="E102" s="2"/>
     </row>
     <row r="103" spans="1:5">
       <c r="E103" s="2"/>
     </row>
-    <row r="104" spans="1:5">
-      <c r="E104" s="2"/>
+    <row r="104" spans="1:5" s="3" customFormat="1">
+      <c r="A104" s="16"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
     </row>
     <row r="105" spans="1:5">
       <c r="E105" s="2"/>
@@ -2071,15 +2113,11 @@
     <row r="111" spans="1:5">
       <c r="E111" s="2"/>
     </row>
-    <row r="112" spans="1:5" s="3" customFormat="1">
-      <c r="A112" s="16"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
-    </row>
-    <row r="113" spans="1:5" s="3" customFormat="1">
-      <c r="A113" s="16"/>
-      <c r="B113" s="1"/>
-      <c r="C113" s="1"/>
+    <row r="112" spans="1:5">
+      <c r="E112" s="2"/>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="E113" s="2"/>
     </row>
     <row r="114" spans="1:5" s="3" customFormat="1">
       <c r="A114" s="16"/>
@@ -2101,42 +2139,46 @@
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="1:5">
-      <c r="E118" s="2"/>
+    <row r="118" spans="1:5" s="3" customFormat="1">
+      <c r="A118" s="16"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
     </row>
     <row r="119" spans="1:5" s="3" customFormat="1">
       <c r="A119" s="16"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
     </row>
-    <row r="120" spans="1:5" s="3" customFormat="1">
-      <c r="A120" s="16"/>
-      <c r="B120" s="1"/>
-      <c r="C120" s="1"/>
-    </row>
-    <row r="121" spans="1:5">
-      <c r="E121" s="2"/>
+    <row r="120" spans="1:5">
+      <c r="E120" s="2"/>
+    </row>
+    <row r="121" spans="1:5" s="3" customFormat="1">
+      <c r="A121" s="16"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="1"/>
     </row>
     <row r="122" spans="1:5" s="3" customFormat="1">
       <c r="A122" s="16"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
     </row>
-    <row r="123" spans="1:5" s="3" customFormat="1">
-      <c r="A123" s="16"/>
-      <c r="B123" s="1"/>
-      <c r="C123" s="1"/>
+    <row r="123" spans="1:5">
+      <c r="E123" s="2"/>
     </row>
     <row r="124" spans="1:5" s="3" customFormat="1">
       <c r="A124" s="16"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
     </row>
-    <row r="125" spans="1:5">
-      <c r="E125" s="2"/>
-    </row>
-    <row r="126" spans="1:5">
-      <c r="E126" s="2"/>
+    <row r="125" spans="1:5" s="3" customFormat="1">
+      <c r="A125" s="16"/>
+      <c r="B125" s="1"/>
+      <c r="C125" s="1"/>
+    </row>
+    <row r="126" spans="1:5" s="3" customFormat="1">
+      <c r="A126" s="16"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
     </row>
     <row r="127" spans="1:5">
       <c r="E127" s="2"/>
@@ -2147,16 +2189,16 @@
     <row r="129" spans="1:5">
       <c r="E129" s="2"/>
     </row>
-    <row r="130" spans="1:5" s="3" customFormat="1">
-      <c r="A130" s="16"/>
-      <c r="B130" s="1"/>
-      <c r="C130" s="1"/>
+    <row r="130" spans="1:5">
+      <c r="E130" s="2"/>
     </row>
     <row r="131" spans="1:5">
       <c r="E131" s="2"/>
     </row>
-    <row r="132" spans="1:5">
-      <c r="E132" s="2"/>
+    <row r="132" spans="1:5" s="3" customFormat="1">
+      <c r="A132" s="16"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
     </row>
     <row r="133" spans="1:5">
       <c r="E133" s="2"/>
@@ -2164,26 +2206,24 @@
     <row r="134" spans="1:5">
       <c r="E134" s="2"/>
     </row>
-    <row r="135" spans="1:5" s="3" customFormat="1">
-      <c r="A135" s="16"/>
-      <c r="B135" s="1"/>
-      <c r="C135" s="1"/>
-    </row>
-    <row r="136" spans="1:5" s="3" customFormat="1">
-      <c r="A136" s="16"/>
-      <c r="B136" s="1"/>
-      <c r="C136" s="1"/>
-    </row>
-    <row r="137" spans="1:5" s="5" customFormat="1">
-      <c r="A137" s="15"/>
+    <row r="135" spans="1:5">
+      <c r="E135" s="2"/>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="E136" s="2"/>
+    </row>
+    <row r="137" spans="1:5" s="3" customFormat="1">
+      <c r="A137" s="16"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
     </row>
-    <row r="138" spans="1:5">
-      <c r="E138" s="2"/>
-    </row>
-    <row r="139" spans="1:5" s="3" customFormat="1">
-      <c r="A139" s="16"/>
+    <row r="138" spans="1:5" s="3" customFormat="1">
+      <c r="A138" s="16"/>
+      <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
+    </row>
+    <row r="139" spans="1:5" s="5" customFormat="1">
+      <c r="A139" s="15"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
     </row>
@@ -2203,10 +2243,8 @@
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
     </row>
-    <row r="144" spans="1:5" s="3" customFormat="1">
-      <c r="A144" s="16"/>
-      <c r="B144" s="1"/>
-      <c r="C144" s="1"/>
+    <row r="144" spans="1:5">
+      <c r="E144" s="2"/>
     </row>
     <row r="145" spans="1:5" s="3" customFormat="1">
       <c r="A145" s="16"/>
@@ -2218,8 +2256,10 @@
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
     </row>
-    <row r="147" spans="1:5">
-      <c r="E147" s="2"/>
+    <row r="147" spans="1:5" s="3" customFormat="1">
+      <c r="A147" s="16"/>
+      <c r="B147" s="1"/>
+      <c r="C147" s="1"/>
     </row>
     <row r="148" spans="1:5" s="3" customFormat="1">
       <c r="A148" s="16"/>
@@ -2229,18 +2269,16 @@
     <row r="149" spans="1:5">
       <c r="E149" s="2"/>
     </row>
-    <row r="150" spans="1:5">
-      <c r="E150" s="2"/>
-    </row>
-    <row r="151" spans="1:5" s="3" customFormat="1">
-      <c r="A151" s="16"/>
-      <c r="B151" s="1"/>
-      <c r="C151" s="1"/>
-    </row>
-    <row r="152" spans="1:5" s="3" customFormat="1">
-      <c r="A152" s="16"/>
-      <c r="B152" s="1"/>
-      <c r="C152" s="1"/>
+    <row r="150" spans="1:5" s="3" customFormat="1">
+      <c r="A150" s="16"/>
+      <c r="B150" s="1"/>
+      <c r="C150" s="1"/>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="E151" s="2"/>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="E152" s="2"/>
     </row>
     <row r="153" spans="1:5" s="3" customFormat="1">
       <c r="A153" s="16"/>
@@ -2297,30 +2335,34 @@
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
     </row>
-    <row r="164" spans="1:5">
-      <c r="E164" s="2"/>
-    </row>
-    <row r="165" spans="1:5">
-      <c r="E165" s="2"/>
+    <row r="164" spans="1:5" s="3" customFormat="1">
+      <c r="A164" s="16"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="1"/>
+    </row>
+    <row r="165" spans="1:5" s="3" customFormat="1">
+      <c r="A165" s="16"/>
+      <c r="B165" s="1"/>
+      <c r="C165" s="1"/>
     </row>
     <row r="166" spans="1:5">
       <c r="E166" s="2"/>
     </row>
-    <row r="167" spans="1:5" s="3" customFormat="1">
-      <c r="A167" s="16"/>
-      <c r="B167" s="1"/>
-      <c r="C167" s="1"/>
-    </row>
-    <row r="168" spans="1:5" s="3" customFormat="1">
-      <c r="A168" s="16"/>
-      <c r="B168" s="1"/>
-      <c r="C168" s="1"/>
-    </row>
-    <row r="169" spans="1:5">
-      <c r="E169" s="2"/>
-    </row>
-    <row r="170" spans="1:5">
-      <c r="E170" s="2"/>
+    <row r="167" spans="1:5">
+      <c r="E167" s="2"/>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="E168" s="2"/>
+    </row>
+    <row r="169" spans="1:5" s="3" customFormat="1">
+      <c r="A169" s="16"/>
+      <c r="B169" s="1"/>
+      <c r="C169" s="1"/>
+    </row>
+    <row r="170" spans="1:5" s="3" customFormat="1">
+      <c r="A170" s="16"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
     </row>
     <row r="171" spans="1:5">
       <c r="E171" s="2"/>
@@ -2331,23 +2373,21 @@
     <row r="173" spans="1:5">
       <c r="E173" s="2"/>
     </row>
-    <row r="174" spans="1:5" s="3" customFormat="1">
-      <c r="A174" s="16"/>
-      <c r="B174" s="1"/>
-      <c r="C174" s="1"/>
-    </row>
-    <row r="175" spans="1:5" s="3" customFormat="1">
-      <c r="A175" s="16"/>
-      <c r="B175" s="1"/>
-      <c r="C175" s="1"/>
-    </row>
-    <row r="176" spans="1:5" s="6" customFormat="1">
-      <c r="A176" s="17"/>
+    <row r="174" spans="1:5">
+      <c r="E174" s="2"/>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="E175" s="2"/>
+    </row>
+    <row r="176" spans="1:5" s="3" customFormat="1">
+      <c r="A176" s="16"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
     </row>
-    <row r="177" spans="1:5">
-      <c r="E177" s="2"/>
+    <row r="177" spans="1:5" s="3" customFormat="1">
+      <c r="A177" s="16"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="1"/>
     </row>
     <row r="178" spans="1:5" s="6" customFormat="1">
       <c r="A178" s="17"/>
@@ -2357,26 +2397,28 @@
     <row r="179" spans="1:5">
       <c r="E179" s="2"/>
     </row>
-    <row r="180" spans="1:5" s="3" customFormat="1">
-      <c r="A180" s="16"/>
+    <row r="180" spans="1:5" s="6" customFormat="1">
+      <c r="A180" s="17"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
     </row>
-    <row r="181" spans="1:5" s="3" customFormat="1">
-      <c r="A181" s="16"/>
-      <c r="B181" s="1"/>
-      <c r="C181" s="1"/>
+    <row r="181" spans="1:5">
+      <c r="E181" s="2"/>
     </row>
     <row r="182" spans="1:5" s="3" customFormat="1">
       <c r="A182" s="16"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
     </row>
-    <row r="183" spans="1:5">
-      <c r="E183" s="2"/>
-    </row>
-    <row r="184" spans="1:5">
-      <c r="E184" s="2"/>
+    <row r="183" spans="1:5" s="3" customFormat="1">
+      <c r="A183" s="16"/>
+      <c r="B183" s="1"/>
+      <c r="C183" s="1"/>
+    </row>
+    <row r="184" spans="1:5" s="3" customFormat="1">
+      <c r="A184" s="16"/>
+      <c r="B184" s="1"/>
+      <c r="C184" s="1"/>
     </row>
     <row r="185" spans="1:5">
       <c r="E185" s="2"/>
@@ -2384,15 +2426,11 @@
     <row r="186" spans="1:5">
       <c r="E186" s="2"/>
     </row>
-    <row r="187" spans="1:5" s="3" customFormat="1">
-      <c r="A187" s="16"/>
-      <c r="B187" s="1"/>
-      <c r="C187" s="1"/>
-    </row>
-    <row r="188" spans="1:5" s="3" customFormat="1">
-      <c r="A188" s="16"/>
-      <c r="B188" s="1"/>
-      <c r="C188" s="1"/>
+    <row r="187" spans="1:5">
+      <c r="E187" s="2"/>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="E188" s="2"/>
     </row>
     <row r="189" spans="1:5" s="3" customFormat="1">
       <c r="A189" s="16"/>
@@ -2429,46 +2467,50 @@
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
     </row>
-    <row r="196" spans="1:5">
-      <c r="E196" s="2"/>
-    </row>
-    <row r="197" spans="1:5">
-      <c r="E197" s="2"/>
+    <row r="196" spans="1:5" s="3" customFormat="1">
+      <c r="A196" s="16"/>
+      <c r="B196" s="1"/>
+      <c r="C196" s="1"/>
+    </row>
+    <row r="197" spans="1:5" s="3" customFormat="1">
+      <c r="A197" s="16"/>
+      <c r="B197" s="1"/>
+      <c r="C197" s="1"/>
     </row>
     <row r="198" spans="1:5">
       <c r="E198" s="2"/>
     </row>
-    <row r="199" spans="1:5" s="3" customFormat="1">
-      <c r="A199" s="16"/>
-      <c r="B199" s="1"/>
-      <c r="C199" s="1"/>
-    </row>
-    <row r="200" spans="1:5" s="3" customFormat="1">
-      <c r="A200" s="16"/>
-      <c r="B200" s="1"/>
-      <c r="C200" s="1"/>
-    </row>
-    <row r="201" spans="1:5">
-      <c r="E201" s="2"/>
-    </row>
-    <row r="202" spans="1:5">
-      <c r="E202" s="2"/>
-    </row>
-    <row r="203" spans="1:5" s="6" customFormat="1">
-      <c r="A203" s="17"/>
-      <c r="B203" s="1"/>
-      <c r="C203" s="1"/>
-    </row>
-    <row r="204" spans="1:5" s="6" customFormat="1">
-      <c r="A204" s="17"/>
-      <c r="B204" s="1"/>
-      <c r="C204" s="1"/>
-    </row>
-    <row r="205" spans="1:5">
-      <c r="E205" s="2"/>
-    </row>
-    <row r="206" spans="1:5">
-      <c r="E206" s="2"/>
+    <row r="199" spans="1:5">
+      <c r="E199" s="2"/>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="E200" s="2"/>
+    </row>
+    <row r="201" spans="1:5" s="3" customFormat="1">
+      <c r="A201" s="16"/>
+      <c r="B201" s="1"/>
+      <c r="C201" s="1"/>
+    </row>
+    <row r="202" spans="1:5" s="3" customFormat="1">
+      <c r="A202" s="16"/>
+      <c r="B202" s="1"/>
+      <c r="C202" s="1"/>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="E203" s="2"/>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="E204" s="2"/>
+    </row>
+    <row r="205" spans="1:5" s="6" customFormat="1">
+      <c r="A205" s="17"/>
+      <c r="B205" s="1"/>
+      <c r="C205" s="1"/>
+    </row>
+    <row r="206" spans="1:5" s="6" customFormat="1">
+      <c r="A206" s="17"/>
+      <c r="B206" s="1"/>
+      <c r="C206" s="1"/>
     </row>
     <row r="207" spans="1:5">
       <c r="E207" s="2"/>
@@ -2479,34 +2521,30 @@
     <row r="209" spans="1:5">
       <c r="E209" s="2"/>
     </row>
-    <row r="210" spans="1:5" s="3" customFormat="1">
-      <c r="A210" s="16"/>
-      <c r="B210" s="1"/>
-      <c r="C210" s="1"/>
-    </row>
-    <row r="211" spans="1:5" s="3" customFormat="1">
-      <c r="A211" s="16"/>
-      <c r="B211" s="1"/>
-      <c r="C211" s="1"/>
-    </row>
-    <row r="212" spans="1:5">
-      <c r="E212" s="2"/>
-    </row>
-    <row r="213" spans="1:5">
-      <c r="E213" s="2"/>
-    </row>
-    <row r="214" spans="1:5" s="3" customFormat="1">
-      <c r="A214" s="16"/>
-      <c r="B214" s="1"/>
-      <c r="C214" s="1"/>
-    </row>
-    <row r="215" spans="1:5" s="3" customFormat="1">
-      <c r="A215" s="16"/>
-      <c r="B215" s="1"/>
-      <c r="C215" s="1"/>
-    </row>
-    <row r="216" spans="1:5" s="5" customFormat="1">
-      <c r="A216" s="15"/>
+    <row r="210" spans="1:5">
+      <c r="E210" s="2"/>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="E211" s="2"/>
+    </row>
+    <row r="212" spans="1:5" s="3" customFormat="1">
+      <c r="A212" s="16"/>
+      <c r="B212" s="1"/>
+      <c r="C212" s="1"/>
+    </row>
+    <row r="213" spans="1:5" s="3" customFormat="1">
+      <c r="A213" s="16"/>
+      <c r="B213" s="1"/>
+      <c r="C213" s="1"/>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="E214" s="2"/>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="E215" s="2"/>
+    </row>
+    <row r="216" spans="1:5" s="3" customFormat="1">
+      <c r="A216" s="16"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
     </row>
@@ -2515,36 +2553,36 @@
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
     </row>
-    <row r="218" spans="1:5">
-      <c r="E218" s="2"/>
+    <row r="218" spans="1:5" s="5" customFormat="1">
+      <c r="A218" s="15"/>
+      <c r="B218" s="1"/>
+      <c r="C218" s="1"/>
     </row>
     <row r="219" spans="1:5" s="3" customFormat="1">
       <c r="A219" s="16"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
     </row>
-    <row r="220" spans="1:5" s="3" customFormat="1">
-      <c r="A220" s="16"/>
-      <c r="B220" s="1"/>
-      <c r="C220" s="1"/>
+    <row r="220" spans="1:5">
+      <c r="E220" s="2"/>
     </row>
     <row r="221" spans="1:5" s="3" customFormat="1">
       <c r="A221" s="16"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
     </row>
-    <row r="222" spans="1:5">
-      <c r="E222" s="2"/>
+    <row r="222" spans="1:5" s="3" customFormat="1">
+      <c r="A222" s="16"/>
+      <c r="B222" s="1"/>
+      <c r="C222" s="1"/>
     </row>
     <row r="223" spans="1:5" s="3" customFormat="1">
       <c r="A223" s="16"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
     </row>
-    <row r="224" spans="1:5" s="3" customFormat="1">
-      <c r="A224" s="16"/>
-      <c r="B224" s="1"/>
-      <c r="C224" s="1"/>
+    <row r="224" spans="1:5">
+      <c r="E224" s="2"/>
     </row>
     <row r="225" spans="1:5" s="3" customFormat="1">
       <c r="A225" s="16"/>
@@ -2571,30 +2609,34 @@
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
     </row>
-    <row r="230" spans="1:5">
-      <c r="E230" s="2"/>
-    </row>
-    <row r="231" spans="1:5">
-      <c r="E231" s="2"/>
-    </row>
-    <row r="232" spans="1:5" s="6" customFormat="1">
-      <c r="A232" s="17"/>
-      <c r="B232" s="1"/>
-      <c r="C232" s="1"/>
+    <row r="230" spans="1:5" s="3" customFormat="1">
+      <c r="A230" s="16"/>
+      <c r="B230" s="1"/>
+      <c r="C230" s="1"/>
+    </row>
+    <row r="231" spans="1:5" s="3" customFormat="1">
+      <c r="A231" s="16"/>
+      <c r="B231" s="1"/>
+      <c r="C231" s="1"/>
+    </row>
+    <row r="232" spans="1:5">
+      <c r="E232" s="2"/>
     </row>
     <row r="233" spans="1:5">
       <c r="E233" s="2"/>
     </row>
-    <row r="234" spans="1:5" s="3" customFormat="1">
-      <c r="A234" s="16"/>
+    <row r="234" spans="1:5" s="6" customFormat="1">
+      <c r="A234" s="17"/>
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
     </row>
     <row r="235" spans="1:5">
       <c r="E235" s="2"/>
     </row>
-    <row r="236" spans="1:5">
-      <c r="E236" s="2"/>
+    <row r="236" spans="1:5" s="3" customFormat="1">
+      <c r="A236" s="16"/>
+      <c r="B236" s="1"/>
+      <c r="C236" s="1"/>
     </row>
     <row r="237" spans="1:5">
       <c r="E237" s="2"/>
@@ -2703,6 +2745,12 @@
     </row>
     <row r="272" spans="5:5">
       <c r="E272" s="2"/>
+    </row>
+    <row r="273" spans="5:5">
+      <c r="E273" s="2"/>
+    </row>
+    <row r="274" spans="5:5">
+      <c r="E274" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A2:XFD1048576">
@@ -2711,15 +2759,15 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E36:E40" r:id="rId1" location="Facility" display="Result_AdverseEventsLabel"/>
+    <hyperlink ref="E38:E42" r:id="rId1" location="Facility" display="Result_AdverseEventsLabel"/>
     <hyperlink ref="E24" r:id="rId2" location="IntDesign"/>
     <hyperlink ref="E21" r:id="rId3" location="Investigators"/>
     <hyperlink ref="E26" r:id="rId4" location="Keywords"/>
-    <hyperlink ref="E34" r:id="rId5" location="StudyOfficials"/>
+    <hyperlink ref="E36" r:id="rId5" location="StudyOfficials"/>
     <hyperlink ref="E27" r:id="rId6" location="Links"/>
-    <hyperlink ref="E41" r:id="rId7" location="LeadSponsor"/>
-    <hyperlink ref="E38" r:id="rId8" location="Result_CertainAgreementLabel"/>
-    <hyperlink ref="E39" r:id="rId9" location="Result_PointOfContactLabel"/>
+    <hyperlink ref="E43" r:id="rId7" location="LeadSponsor"/>
+    <hyperlink ref="E40" r:id="rId8" location="Result_CertainAgreementLabel"/>
+    <hyperlink ref="E41" r:id="rId9" location="Result_PointOfContactLabel"/>
     <hyperlink ref="E11" r:id="rId10" location="crossref"/>
     <hyperlink ref="E4" r:id="rId11" location="BriefSummary"/>
     <hyperlink ref="E19" r:id="rId12" location="Facility"/>
@@ -2731,22 +2779,21 @@
     <hyperlink ref="E20" r:id="rId18" location="FacilityContact"/>
     <hyperlink ref="E22" r:id="rId19" location="SecondaryIds"/>
     <hyperlink ref="E23" r:id="rId20" location="InterventionOtherName"/>
-    <hyperlink ref="E40" r:id="rId21" location="PopFlowArmGroup"/>
+    <hyperlink ref="E42" r:id="rId21" location="PopFlowArmGroup"/>
     <hyperlink ref="E2" r:id="rId22" location="Result_Baseline_ArmGroup_numUnitsAnalyzed"/>
-    <hyperlink ref="E35" r:id="rId23" location="Result_ParticipantFlowLabel"/>
+    <hyperlink ref="E37" r:id="rId23" location="Result_ParticipantFlowLabel"/>
     <hyperlink ref="E17" r:id="rId24" location="NotCompleted"/>
-    <hyperlink ref="E28" r:id="rId25" location="MilestoneName"/>
-    <hyperlink ref="E31" r:id="rId26" location="OutcomeData"/>
-    <hyperlink ref="E36" r:id="rId27" location="Result_AdverseEventsLabel"/>
-    <hyperlink ref="E33" r:id="rId28" location="Result_Outcome_MeasureImg"/>
-    <hyperlink ref="E30" r:id="rId29" location="GroupSelection"/>
-    <hyperlink ref="E29" r:id="rId30" location="Result_Outcome_Analysis"/>
-    <hyperlink ref="E32" r:id="rId31" location="Result_Outcome_MeasureLabel"/>
+    <hyperlink ref="E30" r:id="rId25" location="MilestoneName"/>
+    <hyperlink ref="E33" r:id="rId26" location="OutcomeData"/>
+    <hyperlink ref="E38" r:id="rId27" location="Result_AdverseEventsLabel"/>
+    <hyperlink ref="E35" r:id="rId28" location="Result_Outcome_MeasureImg"/>
+    <hyperlink ref="E32" r:id="rId29" location="GroupSelection"/>
+    <hyperlink ref="E31" r:id="rId30" location="Result_Outcome_Analysis"/>
+    <hyperlink ref="E34" r:id="rId31" location="Result_Outcome_MeasureLabel"/>
     <hyperlink ref="E25" r:id="rId32" location="IPDSharing"/>
     <hyperlink ref="E16" r:id="rId33" location="DocumentUpload"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId34"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
add proj_tag_study_characteristics tables to the Tables table.
</commit_message>
<xml_diff>
--- a/public/documentation/aact_tables.xlsx
+++ b/public/documentation/aact_tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tibbs001/work/aact-admin-1/public/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3B1EB9-D097-B246-97B6-A8BE6D44686D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080654B1-4A24-6D43-9100-2CE62FA55BD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="460" windowWidth="24800" windowHeight="15300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="159">
   <si>
     <t>eligibilities</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -960,6 +960,33 @@
       </rPr>
       <t>roups</t>
     </r>
+  </si>
+  <si>
+    <t>oncology_studies</t>
+  </si>
+  <si>
+    <t>analyzed_studies</t>
+  </si>
+  <si>
+    <t>proj_tag_study_characteristics</t>
+  </si>
+  <si>
+    <t>Trials determined to be oncology related for the purpose of the Study Characteristics investigation.</t>
+  </si>
+  <si>
+    <t>Trials determined to be mental health related for the purpose of the Study Characteristics investigation.</t>
+  </si>
+  <si>
+    <t>Trials determined to be cardiovascular related for the purpose of the Study Characteristics investigation.</t>
+  </si>
+  <si>
+    <t>mental_health_studies</t>
+  </si>
+  <si>
+    <t>cardiovascular_studies</t>
+  </si>
+  <si>
+    <t>Table of terms determined to be either mental health, oncology or cardiovascular-related by a team of Duke clinicians. The source of the terms is the 2010 MeSH thesaurus as well as free-text terms/phrases used to identify interventional studies registered in ClinicalTrials.gov between 2007 and 2010.</t>
   </si>
 </sst>
 </file>
@@ -1566,13 +1593,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="2"/>
+    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="35.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="62" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" style="1" customWidth="1"/>
@@ -2527,7 +2554,7 @@
         <v>18</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>5</v>
+        <v>151</v>
       </c>
       <c r="C49" s="20" t="s">
         <v>27</v>
@@ -2539,19 +2566,65 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="C50" s="21"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>154</v>
+      </c>
       <c r="D51" s="2"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>155</v>
+      </c>
       <c r="D52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D53" s="2"/>
+    <row r="53" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add Project to the last column of the spreadsheet for the new study characteristics project.
</commit_message>
<xml_diff>
--- a/public/documentation/aact_tables.xlsx
+++ b/public/documentation/aact_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tibbs001/work/aact-admin-1/public/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080654B1-4A24-6D43-9100-2CE62FA55BD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB393CF7-81D8-564C-895E-75FF1D4463A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1780" yWindow="460" windowWidth="24800" windowHeight="15300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="159">
   <si>
     <t>eligibilities</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1594,7 +1594,7 @@
   <dimension ref="A1:G273"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2593,7 +2593,12 @@
       <c r="C51" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="D51" s="2"/>
+      <c r="D51" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2606,7 +2611,12 @@
       <c r="C52" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="D52" s="2"/>
+      <c r="D52" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" ht="85" x14ac:dyDescent="0.2">

</xml_diff>